<commit_message>
pandas and numpy logic fixed
</commit_message>
<xml_diff>
--- a/app/backend/2025_11_07_Friday_Sermon_KM5_120642_206380_ENG.xlsx
+++ b/app/backend/2025_11_07_Friday_Sermon_KM5_120642_206380_ENG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m9/Documents/personal_programming/python/projects/gpt/app/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CC3B9C-8489-DC4D-A2A5-26C6A1D624DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276BFE0A-013E-E54B-B7FF-C460738BD7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -9615,8 +9615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="C516" sqref="C516"/>
+    <sheetView tabSelected="1" topLeftCell="A500" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D513" sqref="D513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>